<commit_message>
Elena got our tests to pass.
</commit_message>
<xml_diff>
--- a/data/ClueLayout306.xlsx
+++ b/data/ClueLayout306.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/170d6889d8d02b02/Documents_1D/Education/_Mines/CSCI306/Classes/Clue Material/ClueInitFiles/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ecore/Documents/Colorado School of Mines/2021-2022 Junior Year/CSCI 306/Clue/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1170" documentId="8_{9B645E34-7536-42D9-BF6C-9EF036B3BE1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5DE63DE4-27C8-44E8-B204-76D3DD946929}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DBF327-14CA-5941-BFA0-858822F0DE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="2115" windowWidth="25455" windowHeight="12870" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19240" yWindow="500" windowWidth="16600" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" ClueLayout" sheetId="1" r:id="rId1"/>
@@ -1155,13 +1155,13 @@
       <selection activeCell="AD15" sqref="AD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="24" width="3.7109375" customWidth="1"/>
-    <col min="25" max="25" width="4.5703125" customWidth="1"/>
+    <col min="1" max="24" width="3.6640625" customWidth="1"/>
+    <col min="25" max="25" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B1" s="13">
         <v>0</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -3160,17 +3160,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
     </row>
   </sheetData>
@@ -3184,16 +3184,16 @@
   <dimension ref="A1:AA30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="24" width="3.7109375" customWidth="1"/>
-    <col min="25" max="25" width="3.42578125" customWidth="1"/>
+    <col min="1" max="24" width="3.6640625" customWidth="1"/>
+    <col min="25" max="25" width="3.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B1" s="13">
         <v>0</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -4748,7 +4748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -5133,7 +5133,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -5210,17 +5210,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
     </row>
   </sheetData>
@@ -5236,13 +5236,13 @@
       <selection activeCell="AC17" sqref="AC17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="23" width="3.7109375" customWidth="1"/>
-    <col min="24" max="24" width="4.5703125" customWidth="1"/>
+    <col min="1" max="23" width="3.6640625" customWidth="1"/>
+    <col min="24" max="24" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -5316,7 +5316,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -5464,7 +5464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>12</v>
       </c>
@@ -5538,7 +5538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -5612,7 +5612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>1</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>2</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>2</v>
       </c>
@@ -5982,7 +5982,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>5</v>
       </c>
@@ -6056,7 +6056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>5</v>
       </c>
@@ -6130,7 +6130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
@@ -6204,7 +6204,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>9</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>9</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>9</v>
       </c>
@@ -6426,7 +6426,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>9</v>
       </c>
@@ -6500,7 +6500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>5</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>1</v>
       </c>
@@ -6648,7 +6648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>5</v>
       </c>
@@ -6722,7 +6722,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>0</v>
       </c>
@@ -6796,7 +6796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>0</v>
       </c>
@@ -6870,7 +6870,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>0</v>
       </c>
@@ -6944,7 +6944,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>0</v>
       </c>
@@ -7018,7 +7018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>5</v>
       </c>
@@ -7092,7 +7092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="Y26" s="3"/>
     </row>
   </sheetData>

</xml_diff>